<commit_message>
corrected initial code and added implementation for 7 test cases
</commit_message>
<xml_diff>
--- a/JRI_AUTOMATION_7AM_IST/src/test/resources/testdata/JRI_TestCases_Practice.xlsx
+++ b/JRI_AUTOMATION_7AM_IST/src/test/resources/testdata/JRI_TestCases_Practice.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17670" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="1425"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="3" r:id="rId1"/>
     <sheet name="TestCase" sheetId="1" r:id="rId2"/>
     <sheet name="TestData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1:F11"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:F2"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataSignature="AMtx7mgF78/a9H+gPNq346+/pi9hfI337Q=="/>
@@ -759,7 +759,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="23">
     <font>
       <sz val="11"/>
@@ -1289,6 +1289,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1489,10 +1497,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -2584,10 +2592,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -30127,10 +30135,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>